<commit_message>
update book borrow API
</commit_message>
<xml_diff>
--- a/document/APIIntroduction.xlsx
+++ b/document/APIIntroduction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\BM-Shinetech\BM-Shinetech\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4B2608-1CAE-40B5-8C68-2C21E65B62B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E8C371-DC89-46B4-9510-0ED684AF82C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>function</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -116,6 +116,62 @@
   </si>
   <si>
     <t>api/bookInfo/getById</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>book borrow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>book borrow list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>api/bookBorrow/query</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>keyword(str), pageSize(int), pageIndex(int), userId(bigint)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">get borrowed book by current user </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>borrow book</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>api/bookBorrow/borrowBook</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bookId(bigint), userId(bigint)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if this book has been borrowed, will return message</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return book</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>api/bookBorrow/returnBook</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if this book has been returned, will return message</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>view book detail info</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -441,19 +497,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="6.5" customWidth="1"/>
     <col min="4" max="4" width="27.125" customWidth="1"/>
     <col min="5" max="5" width="49.25" customWidth="1"/>
-    <col min="6" max="6" width="28.25" customWidth="1"/>
+    <col min="6" max="6" width="44.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -539,6 +596,63 @@
       </c>
       <c r="E6" t="s">
         <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>